<commit_message>
absorbance spectra analysis data table for table 1 and spectra analysis graph for figure 1 were generated
</commit_message>
<xml_diff>
--- a/data/data_spectra.xlsx
+++ b/data/data_spectra.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\mcb-protein_isolation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296D56B2-468D-49B3-AF53-447838897C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706A1162-8683-4FDB-996A-D32C2D46F26C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="med_p1_5" sheetId="1" r:id="rId1"/>
+    <sheet name="raw_data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
   <si>
     <t>Wavelength (nm)</t>
   </si>
@@ -35,6 +35,22 @@
   </si>
   <si>
     <t>Absorbace P2-4 High</t>
+  </si>
+  <si>
+    <t>Absorbace Filtrate</t>
+  </si>
+  <si>
+    <t>Absorbace S1</t>
+  </si>
+  <si>
+    <t>Absorbace P1</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absorbance and Wavelength Spectra Data 
+</t>
   </si>
 </sst>
 </file>
@@ -66,7 +82,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -89,20 +105,221 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -142,12 +359,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -155,25 +369,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
+              <a:rPr lang="en-US"/>
               <a:t>Spectrum Analysis of Purified RuBisCo  </a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="1400" baseline="0">
-              <a:effectLst/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.18484711286089239"/>
-          <c:y val="3.7037037037037035E-2"/>
-        </c:manualLayout>
-      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -187,12 +388,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx2"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -214,30 +412,36 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>med_p1_5!$B$1</c:f>
+              <c:f>raw_data!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Absorbance P1-5 Med Salt</c:v>
+                  <c:v>Absorbace Filtrate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>med_p1_5!$A$2:$A$42</c:f>
+              <c:f>raw_data!$A$3:$A$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -369,132 +573,132 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>med_p1_5!$B$2:$B$42</c:f>
+              <c:f>raw_data!$B$3:$B$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.14199999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.114</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.1999999999999998E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.7000000000000004E-2</c:v>
+                  <c:v>2.4209999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.34799999999999998</c:v>
+                  <c:v>3.9249999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.216</c:v>
+                  <c:v>4.2430000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3740000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0429999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.65</c:v>
+                  <c:v>4.4279999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.372</c:v>
+                  <c:v>4.1280000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.20599999999999999</c:v>
+                  <c:v>4.4630000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.128</c:v>
+                  <c:v>4.157</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1</c:v>
+                  <c:v>3.8780000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.7999999999999995E-2</c:v>
+                  <c:v>4.26</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.08</c:v>
+                  <c:v>3.895</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.1999999999999995E-2</c:v>
+                  <c:v>3.9039999999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.4000000000000001E-2</c:v>
+                  <c:v>3.9089999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.3999999999999999E-2</c:v>
+                  <c:v>4.008</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.4999999999999998E-2</c:v>
+                  <c:v>3.782</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.9E-2</c:v>
+                  <c:v>3.7069999999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.3000000000000002E-2</c:v>
+                  <c:v>3.694</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.9000000000000001E-2</c:v>
+                  <c:v>3.6970000000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.5000000000000001E-2</c:v>
+                  <c:v>3.5640000000000001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.1999999999999999E-2</c:v>
+                  <c:v>3.5710000000000002</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.9E-2</c:v>
+                  <c:v>3.5590000000000002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.7000000000000001E-2</c:v>
+                  <c:v>3.637</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>3.5379999999999998</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.2999999999999999E-2</c:v>
+                  <c:v>3.54</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.0999999999999999E-2</c:v>
+                  <c:v>3.4510000000000001</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.01</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.9999999999999993E-3</c:v>
+                  <c:v>3.391</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.0000000000000002E-3</c:v>
+                  <c:v>3.5289999999999999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>7.0000000000000001E-3</c:v>
+                  <c:v>3.4169999999999998</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>3.4369999999999998</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>3.4790000000000001</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>3.4609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>3.548</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>3.37</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>3.4990000000000001</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>3.4329999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -502,7 +706,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5FA4-4C37-9099-2BCECE86EBED}"/>
+              <c16:uniqueId val="{00000000-B2A7-4020-976F-A242BF6823A5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -511,30 +715,36 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>med_p1_5!$C$1</c:f>
+              <c:f>raw_data!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Absorbance P2-5 Med</c:v>
+                  <c:v>Absorbace S1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>med_p1_5!$A$2:$A$42</c:f>
+              <c:f>raw_data!$A$3:$A$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -666,132 +876,132 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>med_p1_5!$C$2:$C$42</c:f>
+              <c:f>raw_data!$C$3:$C$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.251</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25700000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.432</c:v>
+                  <c:v>2.57</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.373</c:v>
+                  <c:v>2.7850000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.38400000000000001</c:v>
+                  <c:v>3.0990000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.72</c:v>
+                  <c:v>3.742</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.486</c:v>
+                  <c:v>4.5359999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.02</c:v>
+                  <c:v>4.8899999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.4510000000000001</c:v>
+                  <c:v>3.9990000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.99</c:v>
+                  <c:v>4.17</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.405</c:v>
+                  <c:v>4.6210000000000004</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.097</c:v>
+                  <c:v>3.9009999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.032</c:v>
+                  <c:v>4.0570000000000004</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.079</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.1559999999999999</c:v>
+                  <c:v>4.0620000000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.1990000000000001</c:v>
+                  <c:v>3.9889999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.1539999999999999</c:v>
+                  <c:v>3.9569999999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.99399999999999999</c:v>
+                  <c:v>4.0019999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.75800000000000001</c:v>
+                  <c:v>3.8210000000000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.497</c:v>
+                  <c:v>3.8239999999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.36</c:v>
+                  <c:v>3.8239999999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.28499999999999998</c:v>
+                  <c:v>3.6789999999999998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.254</c:v>
+                  <c:v>3.7080000000000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.23699999999999999</c:v>
+                  <c:v>3.702</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.22500000000000001</c:v>
+                  <c:v>3.7589999999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.21299999999999999</c:v>
+                  <c:v>3.5019999999999998</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.19700000000000001</c:v>
+                  <c:v>3.6930000000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.182</c:v>
+                  <c:v>3.5750000000000002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.16700000000000001</c:v>
+                  <c:v>3.464</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.155</c:v>
+                  <c:v>3.4540000000000002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.14499999999999999</c:v>
+                  <c:v>3.3460000000000001</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.13800000000000001</c:v>
+                  <c:v>3.4279999999999999</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.13200000000000001</c:v>
+                  <c:v>3.472</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.127</c:v>
+                  <c:v>3.4020000000000001</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.121</c:v>
+                  <c:v>3.302</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.11600000000000001</c:v>
+                  <c:v>3.55</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.111</c:v>
+                  <c:v>3.4340000000000002</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.105</c:v>
+                  <c:v>3.4529999999999998</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9.9000000000000005E-2</c:v>
+                  <c:v>3.4860000000000002</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>9.4E-2</c:v>
+                  <c:v>3.4460000000000002</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>8.8999999999999996E-2</c:v>
+                  <c:v>3.3820000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -799,7 +1009,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5FA4-4C37-9099-2BCECE86EBED}"/>
+              <c16:uniqueId val="{00000001-B2A7-4020-976F-A242BF6823A5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -808,30 +1018,36 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>med_p1_5!$D$1</c:f>
+              <c:f>raw_data!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Absorbace P1-5 High</c:v>
+                  <c:v>Absorbace P1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>med_p1_5!$A$2:$A$42</c:f>
+              <c:f>raw_data!$A$3:$A$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -963,132 +1179,132 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>med_p1_5!$D$2:$D$42</c:f>
+              <c:f>raw_data!$D$3:$D$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>6.5000000000000002E-2</c:v>
+                  <c:v>1.512</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14599999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.14599999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19900000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17100000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.41499999999999998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.339</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.778</c:v>
+                  <c:v>4.4690000000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.1789999999999998</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1040000000000001</c:v>
+                  <c:v>4.4160000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.133</c:v>
+                  <c:v>4.6029999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.495</c:v>
+                  <c:v>3.9689999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.20200000000000001</c:v>
+                  <c:v>4.359</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.8000000000000004E-2</c:v>
+                  <c:v>4.1950000000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.2E-2</c:v>
+                  <c:v>4.2590000000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.05</c:v>
+                  <c:v>3.972</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.3999999999999997E-2</c:v>
+                  <c:v>3.8820000000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.6999999999999998E-2</c:v>
+                  <c:v>3.9470000000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.8000000000000001E-2</c:v>
+                  <c:v>3.9609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.7999999999999999E-2</c:v>
+                  <c:v>3.8260000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.2999999999999999E-2</c:v>
+                  <c:v>3.7650000000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.01</c:v>
+                  <c:v>3.718</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.0000000000000002E-3</c:v>
+                  <c:v>3.6190000000000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.0000000000000002E-3</c:v>
+                  <c:v>3.6440000000000001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.0000000000000001E-3</c:v>
+                  <c:v>3.5950000000000002</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.0000000000000001E-3</c:v>
+                  <c:v>3.601</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>3.5910000000000002</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>3.5110000000000001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>3.4790000000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>3.43</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>3.4319999999999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>3.4340000000000002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>3.4420000000000002</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.5289999999999999</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.5329999999999999</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1E-3</c:v>
+                  <c:v>3.4169999999999998</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>3.3769999999999998</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-1E-3</c:v>
+                  <c:v>3.4729999999999999</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-2E-3</c:v>
+                  <c:v>3.3849999999999998</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-3.0000000000000001E-3</c:v>
+                  <c:v>3.266</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-4.0000000000000001E-3</c:v>
+                  <c:v>2.8769999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1096,7 +1312,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-5FA4-4C37-9099-2BCECE86EBED}"/>
+              <c16:uniqueId val="{00000002-B2A7-4020-976F-A242BF6823A5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1105,30 +1321,36 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>med_p1_5!$E$1</c:f>
+              <c:f>raw_data!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Absorbace P2-4 High</c:v>
+                  <c:v>Absorbance P1-5 Med Salt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>med_p1_5!$A$2:$A$42</c:f>
+              <c:f>raw_data!$A$3:$A$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -1260,132 +1482,132 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>med_p1_5!$E$2:$E$42</c:f>
+              <c:f>raw_data!$E$3:$E$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.63900000000000001</c:v>
+                  <c:v>0.14199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.69499999999999995</c:v>
+                  <c:v>0.114</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.85199999999999998</c:v>
+                  <c:v>9.1999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.65200000000000002</c:v>
+                  <c:v>6.7000000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.64300000000000002</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.89300000000000002</c:v>
+                  <c:v>0.34799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.587</c:v>
+                  <c:v>1.216</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2290000000000001</c:v>
+                  <c:v>1.3740000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.7429999999999999</c:v>
+                  <c:v>1.0429999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.117</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.2349999999999999</c:v>
+                  <c:v>0.372</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.1960000000000002</c:v>
+                  <c:v>0.20599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.2469999999999999</c:v>
+                  <c:v>0.128</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.1619999999999999</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.214</c:v>
+                  <c:v>8.7999999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.19</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.2</c:v>
+                  <c:v>7.1999999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.202</c:v>
+                  <c:v>6.4000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.1419999999999999</c:v>
+                  <c:v>5.3999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.044</c:v>
+                  <c:v>4.4999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.9950000000000001</c:v>
+                  <c:v>3.9E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.018</c:v>
+                  <c:v>3.3000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.66600000000000004</c:v>
+                  <c:v>2.9000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.56899999999999995</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.54500000000000004</c:v>
+                  <c:v>2.1999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.53300000000000003</c:v>
+                  <c:v>1.9E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.52200000000000002</c:v>
+                  <c:v>1.7000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.51100000000000001</c:v>
+                  <c:v>1.4999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.496</c:v>
+                  <c:v>1.2999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.48099999999999998</c:v>
+                  <c:v>1.0999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.46400000000000002</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.44900000000000001</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.435</c:v>
+                  <c:v>8.0000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.42099999999999999</c:v>
+                  <c:v>7.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.40699999999999997</c:v>
+                  <c:v>6.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.39200000000000002</c:v>
+                  <c:v>6.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.378</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.36299999999999999</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.34799999999999998</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.33200000000000002</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.317</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1393,12 +1615,922 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000002A-5FA4-4C37-9099-2BCECE86EBED}"/>
+              <c16:uniqueId val="{00000003-B2A7-4020-976F-A242BF6823A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>raw_data!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Absorbance P2-5 Med</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>raw_data!$A$3:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>raw_data!$F$3:$F$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>0.251</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.432</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.373</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.38400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.486</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.4510000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.405</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.097</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.032</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.079</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1559999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.1990000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.1539999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.75800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.497</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.28499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.254</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.23699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.22500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.21299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.19700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.182</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.16700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.155</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.14499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.13800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.13200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.127</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.121</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.11600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.111</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.105</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9.9000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>8.8999999999999996E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B2A7-4020-976F-A242BF6823A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>raw_data!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Absorbace P1-5 High</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>raw_data!$A$3:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>raw_data!$G$3:$G$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>6.5000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.41499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.339</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.778</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1789999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1040000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.133</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.495</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.20200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.8000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.3999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.6999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2E-3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1E-3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-2E-3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-4.0000000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-B2A7-4020-976F-A242BF6823A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>raw_data!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Absorbace P2-4 High</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>raw_data!$A$3:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>raw_data!$H$3:$H$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>0.63900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.69499999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.65200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.64300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.587</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2290000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.7429999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.117</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.2349999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.1960000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.2469999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.1619999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.214</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.19</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.202</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.1419999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.044</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.9950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.018</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.66600000000000004</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.56899999999999995</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.54500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.53300000000000003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.52200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.51100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.496</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.48099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.46400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.44900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.435</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.42099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.40699999999999997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.39200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.378</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.36299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.34799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.33200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.317</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-B2A7-4020-976F-A242BF6823A5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1406,11 +2538,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1385930448"/>
-        <c:axId val="1385929616"/>
+        <c:axId val="812287360"/>
+        <c:axId val="812290272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1385930448"/>
+        <c:axId val="812287360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="400"/>
@@ -1422,7 +2554,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="tx2">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -1439,12 +2571,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx2"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1452,14 +2581,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" i="0" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
+                  <a:rPr lang="en-US"/>
                   <a:t>Wavelength (nm)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1000">
-                  <a:effectLst/>
-                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1476,12 +2600,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx2"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1500,9 +2621,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1516,10 +2637,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1529,12 +2647,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1385929616"/>
+        <c:crossAx val="812290272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1385929616"/>
+        <c:axId val="812290272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1544,7 +2662,7 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:schemeClr val="tx2">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
                 </a:schemeClr>
@@ -1561,12 +2679,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx2"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1574,14 +2689,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" i="0" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
+                  <a:rPr lang="en-US"/>
                   <a:t>Absorbance</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1000">
-                  <a:effectLst/>
-                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1598,12 +2708,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx2"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1620,14 +2727,13 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln>
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1638,10 +2744,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx2"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1651,7 +2754,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1385930448"/>
+        <c:crossAx val="812287360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1664,7 +2767,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1680,10 +2783,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx2"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1711,7 +2811,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="tx2">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1779,35 +2879,29 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1820,7 +2914,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1828,7 +2922,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1836,17 +2930,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
@@ -1855,9 +2946,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
@@ -1880,35 +2970,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="2"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="2"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1920,18 +3010,19 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="2"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
@@ -1940,10 +3031,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1959,21 +3050,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1983,23 +3069,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2008,17 +3093,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2027,14 +3112,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2046,26 +3130,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2079,17 +3157,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -2098,17 +3175,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2117,17 +3194,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="tx2">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2136,27 +3212,24 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -2164,11 +3237,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2176,17 +3257,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -2195,12 +3276,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2209,14 +3287,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2225,10 +3302,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
@@ -2237,20 +3311,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2259,20 +3332,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2282,14 +3351,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2298,23 +3361,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>588111</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>158911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>334945</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>94204</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F47FC933-CEF3-4204-9F8C-82771B4F8126}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43ECD883-7101-4595-B698-5A33F891F1AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2656,735 +3719,1128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="H43" sqref="A1:H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="25.77734375" style="2" customWidth="1"/>
-    <col min="3" max="5" width="25.77734375" customWidth="1"/>
+    <col min="1" max="8" width="25.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H2" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
         <v>200</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.512</v>
+      </c>
+      <c r="E3" s="4">
         <v>0.14199999999999999</v>
       </c>
-      <c r="C2">
+      <c r="F3" s="4">
         <v>0.251</v>
       </c>
-      <c r="D2">
+      <c r="G3" s="4">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E2">
+      <c r="H3" s="12">
         <v>0.63900000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
         <v>205</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3">
         <v>0.114</v>
       </c>
-      <c r="C3">
+      <c r="F4" s="3">
         <v>0.25700000000000001</v>
       </c>
-      <c r="D3">
+      <c r="G4" s="3">
         <v>0.14599999999999999</v>
       </c>
-      <c r="E3">
+      <c r="H4" s="14">
         <v>0.69499999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
         <v>210</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2.57</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="C4">
+      <c r="F5" s="3">
         <v>0.432</v>
       </c>
-      <c r="D4">
+      <c r="G5" s="3">
         <v>0.14599999999999999</v>
       </c>
-      <c r="E4">
+      <c r="H5" s="14">
         <v>0.85199999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="13">
         <v>215</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="3">
+        <v>2.4209999999999998</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2.7850000000000001</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="C5">
+      <c r="F6" s="3">
         <v>0.373</v>
       </c>
-      <c r="D5">
+      <c r="G6" s="3">
         <v>0.19900000000000001</v>
       </c>
-      <c r="E5">
+      <c r="H6" s="14">
         <v>0.65200000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="13">
         <v>220</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3.0990000000000002</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3">
         <v>0.15</v>
       </c>
-      <c r="C6">
+      <c r="F7" s="3">
         <v>0.38400000000000001</v>
       </c>
-      <c r="D6">
+      <c r="G7" s="3">
         <v>0.17100000000000001</v>
       </c>
-      <c r="E6">
+      <c r="H7" s="14">
         <v>0.64300000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="13">
         <v>225</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="3">
+        <v>3.9249999999999998</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3.742</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3">
         <v>0.34799999999999998</v>
       </c>
-      <c r="C7">
+      <c r="F8" s="3">
         <v>0.72</v>
       </c>
-      <c r="D7">
+      <c r="G8" s="3">
         <v>0.41499999999999998</v>
       </c>
-      <c r="E7">
+      <c r="H8" s="14">
         <v>0.89300000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="13">
         <v>230</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="3">
+        <v>4.2430000000000003</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4.5359999999999996</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3">
         <v>1.216</v>
       </c>
-      <c r="C8">
+      <c r="F9" s="3">
         <v>1.486</v>
       </c>
-      <c r="D8">
+      <c r="G9" s="3">
         <v>1.339</v>
       </c>
-      <c r="E8">
+      <c r="H9" s="14">
         <v>1.587</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="13">
         <v>235</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4.4690000000000003</v>
+      </c>
+      <c r="E10" s="3">
         <v>1.3740000000000001</v>
       </c>
-      <c r="C9">
+      <c r="F10" s="3">
         <v>2.02</v>
       </c>
-      <c r="D9">
+      <c r="G10" s="3">
         <v>1.778</v>
       </c>
-      <c r="E9">
+      <c r="H10" s="14">
         <v>2.2290000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
         <v>240</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3.9990000000000001</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="3">
         <v>1.0429999999999999</v>
       </c>
-      <c r="C10">
+      <c r="F11" s="3">
         <v>2.4510000000000001</v>
       </c>
-      <c r="D10">
+      <c r="G11" s="3">
         <v>2.1789999999999998</v>
       </c>
-      <c r="E10">
+      <c r="H11" s="14">
         <v>2.7429999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
         <v>245</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B12" s="3">
+        <v>4.4279999999999999</v>
+      </c>
+      <c r="C12" s="3">
+        <v>4.17</v>
+      </c>
+      <c r="D12" s="3">
+        <v>4.4160000000000004</v>
+      </c>
+      <c r="E12" s="3">
         <v>0.65</v>
       </c>
-      <c r="C11">
+      <c r="F12" s="3">
         <v>1.99</v>
       </c>
-      <c r="D11">
+      <c r="G12" s="3">
         <v>2.1040000000000001</v>
       </c>
-      <c r="E11">
+      <c r="H12" s="14">
         <v>3.117</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="13">
         <v>250</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B13" s="3">
+        <v>4.1280000000000001</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4.6210000000000004</v>
+      </c>
+      <c r="D13" s="3">
+        <v>4.6029999999999998</v>
+      </c>
+      <c r="E13" s="3">
         <v>0.372</v>
       </c>
-      <c r="C12">
+      <c r="F13" s="3">
         <v>1.405</v>
       </c>
-      <c r="D12">
+      <c r="G13" s="3">
         <v>1.133</v>
       </c>
-      <c r="E12">
+      <c r="H13" s="14">
         <v>3.2349999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="13">
         <v>255</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="3">
+        <v>4.4630000000000001</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3.9009999999999998</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3.9689999999999999</v>
+      </c>
+      <c r="E14" s="3">
         <v>0.20599999999999999</v>
       </c>
-      <c r="C13">
+      <c r="F14" s="3">
         <v>1.097</v>
       </c>
-      <c r="D13">
+      <c r="G14" s="3">
         <v>0.495</v>
       </c>
-      <c r="E13">
+      <c r="H14" s="14">
         <v>3.1960000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="13">
         <v>260</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B15" s="3">
+        <v>4.157</v>
+      </c>
+      <c r="C15" s="3">
+        <v>4.0570000000000004</v>
+      </c>
+      <c r="D15" s="3">
+        <v>4.359</v>
+      </c>
+      <c r="E15" s="3">
         <v>0.128</v>
       </c>
-      <c r="C14">
+      <c r="F15" s="3">
         <v>1.032</v>
       </c>
-      <c r="D14">
+      <c r="G15" s="3">
         <v>0.20200000000000001</v>
       </c>
-      <c r="E14">
+      <c r="H15" s="14">
         <v>3.2469999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="13">
         <v>265</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B16" s="3">
+        <v>3.8780000000000001</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3">
+        <v>4.1950000000000003</v>
+      </c>
+      <c r="E16" s="3">
         <v>0.1</v>
       </c>
-      <c r="C15">
+      <c r="F16" s="3">
         <v>1.079</v>
       </c>
-      <c r="D15">
+      <c r="G16" s="3">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="E15">
+      <c r="H16" s="14">
         <v>3.1619999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17" s="13">
         <v>270</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B17" s="3">
+        <v>4.26</v>
+      </c>
+      <c r="C17" s="3">
+        <v>4.0620000000000003</v>
+      </c>
+      <c r="D17" s="3">
+        <v>4.2590000000000003</v>
+      </c>
+      <c r="E17" s="3">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="C16">
+      <c r="F17" s="3">
         <v>1.1559999999999999</v>
       </c>
-      <c r="D16">
+      <c r="G17" s="3">
         <v>6.2E-2</v>
       </c>
-      <c r="E16">
+      <c r="H17" s="14">
         <v>3.214</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A18" s="13">
         <v>275</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B18" s="3">
+        <v>3.895</v>
+      </c>
+      <c r="C18" s="3">
+        <v>3.9889999999999999</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3.972</v>
+      </c>
+      <c r="E18" s="3">
         <v>0.08</v>
       </c>
-      <c r="C17">
+      <c r="F18" s="3">
         <v>1.1990000000000001</v>
       </c>
-      <c r="D17">
+      <c r="G18" s="3">
         <v>0.05</v>
       </c>
-      <c r="E17">
+      <c r="H18" s="14">
         <v>3.19</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A19" s="13">
         <v>280</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B19" s="3">
+        <v>3.9039999999999999</v>
+      </c>
+      <c r="C19" s="3">
+        <v>3.9569999999999999</v>
+      </c>
+      <c r="D19" s="3">
+        <v>3.8820000000000001</v>
+      </c>
+      <c r="E19" s="3">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="C18">
+      <c r="F19" s="3">
         <v>1.1539999999999999</v>
       </c>
-      <c r="D18">
+      <c r="G19" s="3">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="E18">
+      <c r="H19" s="14">
         <v>3.2</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A20" s="13">
         <v>285</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B20" s="3">
+        <v>3.9089999999999998</v>
+      </c>
+      <c r="C20" s="3">
+        <v>4.0019999999999998</v>
+      </c>
+      <c r="D20" s="3">
+        <v>3.9470000000000001</v>
+      </c>
+      <c r="E20" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="C19">
+      <c r="F20" s="3">
         <v>0.99399999999999999</v>
       </c>
-      <c r="D19">
+      <c r="G20" s="3">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="E19">
+      <c r="H20" s="14">
         <v>3.202</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A21" s="13">
         <v>290</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B21" s="3">
+        <v>4.008</v>
+      </c>
+      <c r="C21" s="3">
+        <v>3.8210000000000002</v>
+      </c>
+      <c r="D21" s="3">
+        <v>3.9609999999999999</v>
+      </c>
+      <c r="E21" s="3">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="C20">
+      <c r="F21" s="3">
         <v>0.75800000000000001</v>
       </c>
-      <c r="D20">
+      <c r="G21" s="3">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="E20">
+      <c r="H21" s="14">
         <v>3.1419999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A22" s="13">
         <v>295</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B22" s="3">
+        <v>3.782</v>
+      </c>
+      <c r="C22" s="3">
+        <v>3.8239999999999998</v>
+      </c>
+      <c r="D22" s="3">
+        <v>3.8260000000000001</v>
+      </c>
+      <c r="E22" s="3">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="C21">
+      <c r="F22" s="3">
         <v>0.497</v>
       </c>
-      <c r="D21">
+      <c r="G22" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E21">
+      <c r="H22" s="14">
         <v>3.044</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A23" s="13">
         <v>300</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B23" s="3">
+        <v>3.7069999999999999</v>
+      </c>
+      <c r="C23" s="3">
+        <v>3.8239999999999998</v>
+      </c>
+      <c r="D23" s="3">
+        <v>3.7650000000000001</v>
+      </c>
+      <c r="E23" s="3">
         <v>3.9E-2</v>
       </c>
-      <c r="C22">
+      <c r="F23" s="3">
         <v>0.36</v>
       </c>
-      <c r="D22">
+      <c r="G23" s="3">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="E22">
+      <c r="H23" s="14">
         <v>1.9950000000000001</v>
       </c>
-      <c r="R22" s="3"/>
+      <c r="U23" s="2"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A24" s="13">
         <v>305</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B24" s="3">
+        <v>3.694</v>
+      </c>
+      <c r="C24" s="3">
+        <v>3.6789999999999998</v>
+      </c>
+      <c r="D24" s="3">
+        <v>3.718</v>
+      </c>
+      <c r="E24" s="3">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="C23">
+      <c r="F24" s="3">
         <v>0.28499999999999998</v>
       </c>
-      <c r="D23">
+      <c r="G24" s="3">
         <v>0.01</v>
       </c>
-      <c r="E23">
+      <c r="H24" s="14">
         <v>1.018</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A25" s="13">
         <v>310</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B25" s="3">
+        <v>3.6970000000000001</v>
+      </c>
+      <c r="C25" s="3">
+        <v>3.7080000000000002</v>
+      </c>
+      <c r="D25" s="3">
+        <v>3.6190000000000002</v>
+      </c>
+      <c r="E25" s="3">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="C24">
+      <c r="F25" s="3">
         <v>0.254</v>
       </c>
-      <c r="D24">
+      <c r="G25" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E24">
+      <c r="H25" s="14">
         <v>0.66600000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A26" s="13">
         <v>315</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B26" s="3">
+        <v>3.5640000000000001</v>
+      </c>
+      <c r="C26" s="3">
+        <v>3.702</v>
+      </c>
+      <c r="D26" s="3">
+        <v>3.6440000000000001</v>
+      </c>
+      <c r="E26" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C25">
+      <c r="F26" s="3">
         <v>0.23699999999999999</v>
       </c>
-      <c r="D25">
+      <c r="G26" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E25">
+      <c r="H26" s="14">
         <v>0.56899999999999995</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A27" s="13">
         <v>320</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B27" s="3">
+        <v>3.5710000000000002</v>
+      </c>
+      <c r="C27" s="3">
+        <v>3.7589999999999999</v>
+      </c>
+      <c r="D27" s="3">
+        <v>3.5950000000000002</v>
+      </c>
+      <c r="E27" s="3">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C26">
+      <c r="F27" s="3">
         <v>0.22500000000000001</v>
       </c>
-      <c r="D26">
+      <c r="G27" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E26">
+      <c r="H27" s="14">
         <v>0.54500000000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A28" s="13">
         <v>325</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B28" s="3">
+        <v>3.5590000000000002</v>
+      </c>
+      <c r="C28" s="3">
+        <v>3.5019999999999998</v>
+      </c>
+      <c r="D28" s="3">
+        <v>3.601</v>
+      </c>
+      <c r="E28" s="3">
         <v>1.9E-2</v>
       </c>
-      <c r="C27">
+      <c r="F28" s="3">
         <v>0.21299999999999999</v>
       </c>
-      <c r="D27">
+      <c r="G28" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E27">
+      <c r="H28" s="14">
         <v>0.53300000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A29" s="13">
         <v>330</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B29" s="3">
+        <v>3.637</v>
+      </c>
+      <c r="C29" s="3">
+        <v>3.6930000000000001</v>
+      </c>
+      <c r="D29" s="3">
+        <v>3.5910000000000002</v>
+      </c>
+      <c r="E29" s="3">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="C28">
+      <c r="F29" s="3">
         <v>0.19700000000000001</v>
       </c>
-      <c r="D28">
+      <c r="G29" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="E28">
+      <c r="H29" s="14">
         <v>0.52200000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A30" s="13">
         <v>335</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B30" s="3">
+        <v>3.5379999999999998</v>
+      </c>
+      <c r="C30" s="3">
+        <v>3.5750000000000002</v>
+      </c>
+      <c r="D30" s="3">
+        <v>3.5110000000000001</v>
+      </c>
+      <c r="E30" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="C29">
+      <c r="F30" s="3">
         <v>0.182</v>
       </c>
-      <c r="D29">
+      <c r="G30" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="E29">
+      <c r="H30" s="14">
         <v>0.51100000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A31" s="13">
         <v>340</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B31" s="3">
+        <v>3.54</v>
+      </c>
+      <c r="C31" s="3">
+        <v>3.464</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3.4790000000000001</v>
+      </c>
+      <c r="E31" s="3">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="C30">
+      <c r="F31" s="3">
         <v>0.16700000000000001</v>
       </c>
-      <c r="D30">
+      <c r="G31" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E30">
+      <c r="H31" s="14">
         <v>0.496</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A32" s="13">
         <v>345</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B32" s="3">
+        <v>3.4510000000000001</v>
+      </c>
+      <c r="C32" s="3">
+        <v>3.4540000000000002</v>
+      </c>
+      <c r="D32" s="3">
+        <v>3.43</v>
+      </c>
+      <c r="E32" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="C31">
+      <c r="F32" s="3">
         <v>0.155</v>
       </c>
-      <c r="D31">
+      <c r="G32" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E31">
+      <c r="H32" s="14">
         <v>0.48099999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="13">
         <v>350</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B33" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="C33" s="3">
+        <v>3.3460000000000001</v>
+      </c>
+      <c r="D33" s="3">
+        <v>3.4319999999999999</v>
+      </c>
+      <c r="E33" s="3">
         <v>0.01</v>
       </c>
-      <c r="C32">
+      <c r="F33" s="3">
         <v>0.14499999999999999</v>
       </c>
-      <c r="D32">
+      <c r="G33" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E32">
+      <c r="H33" s="14">
         <v>0.46400000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="13">
         <v>355</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B34" s="3">
+        <v>3.391</v>
+      </c>
+      <c r="C34" s="3">
+        <v>3.4279999999999999</v>
+      </c>
+      <c r="D34" s="3">
+        <v>3.4340000000000002</v>
+      </c>
+      <c r="E34" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="C33">
+      <c r="F34" s="3">
         <v>0.13800000000000001</v>
       </c>
-      <c r="D33">
+      <c r="G34" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E33">
+      <c r="H34" s="14">
         <v>0.44900000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="13">
         <v>360</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B35" s="3">
+        <v>3.5289999999999999</v>
+      </c>
+      <c r="C35" s="3">
+        <v>3.472</v>
+      </c>
+      <c r="D35" s="3">
+        <v>3.4420000000000002</v>
+      </c>
+      <c r="E35" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C34">
+      <c r="F35" s="3">
         <v>0.13200000000000001</v>
       </c>
-      <c r="D34">
+      <c r="G35" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E34">
+      <c r="H35" s="14">
         <v>0.435</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="13">
         <v>365</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B36" s="3">
+        <v>3.4169999999999998</v>
+      </c>
+      <c r="C36" s="3">
+        <v>3.4020000000000001</v>
+      </c>
+      <c r="D36" s="3">
+        <v>3.5289999999999999</v>
+      </c>
+      <c r="E36" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C35">
+      <c r="F36" s="3">
         <v>0.127</v>
       </c>
-      <c r="D35">
+      <c r="G36" s="3">
         <v>2E-3</v>
       </c>
-      <c r="E35">
+      <c r="H36" s="14">
         <v>0.42099999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="13">
         <v>370</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B37" s="3">
+        <v>3.4369999999999998</v>
+      </c>
+      <c r="C37" s="3">
+        <v>3.302</v>
+      </c>
+      <c r="D37" s="3">
+        <v>3.5329999999999999</v>
+      </c>
+      <c r="E37" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C36">
+      <c r="F37" s="3">
         <v>0.121</v>
       </c>
-      <c r="D36">
+      <c r="G37" s="3">
         <v>2E-3</v>
       </c>
-      <c r="E36">
+      <c r="H37" s="14">
         <v>0.40699999999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="13">
         <v>375</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B38" s="3">
+        <v>3.4790000000000001</v>
+      </c>
+      <c r="C38" s="3">
+        <v>3.55</v>
+      </c>
+      <c r="D38" s="3">
+        <v>3.4169999999999998</v>
+      </c>
+      <c r="E38" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C37">
+      <c r="F38" s="3">
         <v>0.11600000000000001</v>
       </c>
-      <c r="D37">
+      <c r="G38" s="3">
         <v>1E-3</v>
       </c>
-      <c r="E37">
+      <c r="H38" s="14">
         <v>0.39200000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="13">
         <v>380</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B39" s="3">
+        <v>3.4609999999999999</v>
+      </c>
+      <c r="C39" s="3">
+        <v>3.4340000000000002</v>
+      </c>
+      <c r="D39" s="3">
+        <v>3.3769999999999998</v>
+      </c>
+      <c r="E39" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C38">
+      <c r="F39" s="3">
         <v>0.111</v>
       </c>
-      <c r="D38">
+      <c r="G39" s="3">
         <v>0</v>
       </c>
-      <c r="E38">
+      <c r="H39" s="14">
         <v>0.378</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="13">
         <v>385</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B40" s="3">
+        <v>3.548</v>
+      </c>
+      <c r="C40" s="3">
+        <v>3.4529999999999998</v>
+      </c>
+      <c r="D40" s="3">
+        <v>3.4729999999999999</v>
+      </c>
+      <c r="E40" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C39">
+      <c r="F40" s="3">
         <v>0.105</v>
       </c>
-      <c r="D39">
+      <c r="G40" s="3">
         <v>-1E-3</v>
       </c>
-      <c r="E39">
+      <c r="H40" s="14">
         <v>0.36299999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="13">
         <v>390</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B41" s="3">
+        <v>3.37</v>
+      </c>
+      <c r="C41" s="3">
+        <v>3.4860000000000002</v>
+      </c>
+      <c r="D41" s="3">
+        <v>3.3849999999999998</v>
+      </c>
+      <c r="E41" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="C40">
+      <c r="F41" s="3">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="D40">
+      <c r="G41" s="3">
         <v>-2E-3</v>
       </c>
-      <c r="E40">
+      <c r="H41" s="14">
         <v>0.34799999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="13">
         <v>395</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B42" s="3">
+        <v>3.4990000000000001</v>
+      </c>
+      <c r="C42" s="3">
+        <v>3.4460000000000002</v>
+      </c>
+      <c r="D42" s="3">
+        <v>3.266</v>
+      </c>
+      <c r="E42" s="3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="C41">
+      <c r="F42" s="3">
         <v>9.4E-2</v>
       </c>
-      <c r="D41">
+      <c r="G42" s="3">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="E41">
+      <c r="H42" s="14">
         <v>0.33200000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
+    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="15">
         <v>400</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B43" s="16">
+        <v>3.4329999999999998</v>
+      </c>
+      <c r="C43" s="16">
+        <v>3.3820000000000001</v>
+      </c>
+      <c r="D43" s="16">
+        <v>2.8769999999999998</v>
+      </c>
+      <c r="E43" s="16">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="C42">
+      <c r="F43" s="16">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="D42">
+      <c r="G43" s="16">
         <v>-4.0000000000000001E-3</v>
       </c>
-      <c r="E42">
+      <c r="H43" s="17">
         <v>0.317</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>